<commit_message>
Remove white spaces in the IG
</commit_message>
<xml_diff>
--- a/tools/anssi/Label EBIOS Risk Manager.xlsx
+++ b/tools/anssi/Label EBIOS Risk Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanabshirali/Desktop/stage MAi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993428E4-9B05-0742-B92F-7C13057353AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B9AD3B-EFAD-C648-B788-9AEF51A07816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="520" windowWidth="28240" windowHeight="15860" activeTab="1" xr2:uid="{C2516E89-280E-5C41-893C-113C1BBD8AF3}"/>
+    <workbookView xWindow="100" yWindow="520" windowWidth="28240" windowHeight="15860" activeTab="2" xr2:uid="{C2516E89-280E-5C41-893C-113C1BBD8AF3}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="510">
   <si>
     <t>ref_id</t>
   </si>
@@ -106,13 +106,7 @@
     <t>fr</t>
   </si>
   <si>
-    <t xml:space="preserve">Standalone </t>
-  </si>
-  <si>
     <t>SaaS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client-Serveur </t>
   </si>
   <si>
     <t>Le logiciel fonctionnant de manière autonome sur une station de travail est soumis aux
@@ -2151,7 +2145,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -2178,7 +2172,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2186,7 +2180,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -2195,7 +2189,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2204,7 +2198,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -2213,7 +2207,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -2231,7 +2225,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -2240,7 +2234,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -2249,7 +2243,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -2258,7 +2252,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -2267,7 +2261,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>18</v>
@@ -2293,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5548FFBD-2E0F-8E4B-9395-B7436C519960}">
   <dimension ref="A1:H232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView topLeftCell="A170" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2308,25 +2302,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" s="10"/>
     </row>
@@ -2339,10 +2333,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2351,111 +2345,111 @@
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2464,27 +2458,27 @@
         <v>2</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2493,27 +2487,27 @@
         <v>2</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2522,83 +2516,83 @@
         <v>2</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C17" s="16">
         <v>4</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C18" s="16">
         <v>4</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C19" s="16">
         <v>4</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C20" s="16">
         <v>4</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2610,10 +2604,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2622,13 +2616,13 @@
         <v>2</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2637,146 +2631,146 @@
         <v>3</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C24">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C25">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C28">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2785,121 +2779,121 @@
         <v>3</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C38">
         <v>4</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2908,160 +2902,160 @@
         <v>3</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E39" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C40">
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C41">
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:7" ht="43" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C42">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C43">
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C44">
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C45">
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G45" s="11"/>
     </row>
     <row r="46" spans="1:7" ht="43" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G46" s="11"/>
     </row>
     <row r="47" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>324</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C47">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>328</v>
-      </c>
       <c r="G47" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3070,172 +3064,172 @@
         <v>3</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C49">
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C50">
         <v>4</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C52">
         <v>4</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C53">
         <v>4</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C54">
         <v>4</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C55">
         <v>4</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C56">
         <v>4</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C57">
         <v>4</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3244,13 +3238,13 @@
         <v>2</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3259,84 +3253,84 @@
         <v>3</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E59" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F59" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C60">
         <v>4</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C61">
         <v>4</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C62">
         <v>4</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C63">
         <v>4</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3345,101 +3339,101 @@
         <v>3</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C65">
         <v>4</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C66">
         <v>4</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C67">
         <v>4</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C68">
         <v>4</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C69">
         <v>4</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3448,81 +3442,81 @@
         <v>3</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C71">
         <v>4</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C72">
         <v>4</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C73">
         <v>4</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C74">
         <v>4</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3531,13 +3525,13 @@
         <v>2</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -3546,339 +3540,339 @@
         <v>3</v>
       </c>
       <c r="D76" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F76" s="21" t="s">
         <v>124</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="F76" s="21" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C77">
         <v>4</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C78">
         <v>4</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C79">
         <v>4</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C80">
         <v>4</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C81">
         <v>4</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C82">
         <v>4</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C83">
         <v>4</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C84">
         <v>4</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C85">
         <v>4</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C86">
         <v>4</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C87">
         <v>4</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C88">
         <v>4</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C89">
         <v>4</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C90">
         <v>4</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G90" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C91">
         <v>4</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C92">
         <v>4</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C93">
         <v>4</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C94">
         <v>4</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C95">
         <v>4</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3887,138 +3881,138 @@
         <v>3</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C97">
         <v>4</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C98">
         <v>4</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G98" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C99">
         <v>4</v>
       </c>
       <c r="D99" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C100">
         <v>4</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C101">
         <v>4</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C102">
         <v>4</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G102" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C103">
         <v>4</v>
       </c>
       <c r="D103" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4027,115 +4021,115 @@
         <v>3</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C105">
         <v>4</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C106">
         <v>4</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C107">
         <v>4</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C108">
         <v>4</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C109">
         <v>4</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C110">
         <v>4</v>
       </c>
       <c r="D110" s="22" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4144,13 +4138,13 @@
         <v>2</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E111" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F111" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4159,118 +4153,118 @@
         <v>3</v>
       </c>
       <c r="D112" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E112" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="F112" s="21" t="s">
         <v>165</v>
-      </c>
-      <c r="E112" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="F112" s="21" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C113">
         <v>4</v>
       </c>
       <c r="D113" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G113" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C114">
         <v>4</v>
       </c>
       <c r="D114" s="23" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C115">
         <v>4</v>
       </c>
       <c r="D115" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C116">
         <v>4</v>
       </c>
       <c r="D116" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C117">
         <v>4</v>
       </c>
       <c r="D117" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C118">
         <v>4</v>
       </c>
       <c r="D118" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="119" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4279,291 +4273,291 @@
         <v>3</v>
       </c>
       <c r="D119" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E119" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F119" s="21" t="s">
         <v>174</v>
-      </c>
-      <c r="E119" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F119" s="21" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C120">
         <v>4</v>
       </c>
       <c r="D120" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C121">
         <v>5</v>
       </c>
       <c r="D121" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C122">
         <v>5</v>
       </c>
       <c r="D122" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C123">
         <v>5</v>
       </c>
       <c r="D123" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C124">
         <v>4</v>
       </c>
       <c r="D124" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C125">
         <v>4</v>
       </c>
       <c r="D125" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C126">
         <v>4</v>
       </c>
       <c r="D126" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C127">
         <v>4</v>
       </c>
       <c r="D127" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C128">
         <v>4</v>
       </c>
       <c r="D128" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C129">
         <v>4</v>
       </c>
       <c r="D129" s="23" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C130">
         <v>4</v>
       </c>
       <c r="D130" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C131">
         <v>4</v>
       </c>
       <c r="D131" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C132">
         <v>4</v>
       </c>
       <c r="D132" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C133">
         <v>4</v>
       </c>
       <c r="D133" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C134">
         <v>4</v>
       </c>
       <c r="D134" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C135">
         <v>4</v>
       </c>
       <c r="D135" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="136" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4572,13 +4566,13 @@
         <v>2</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E136" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F136" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="137" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4587,84 +4581,84 @@
         <v>3</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E137" s="17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F137" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C138">
         <v>4</v>
       </c>
       <c r="D138" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F138" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G138" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C139">
         <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F139" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C140">
         <v>4</v>
       </c>
       <c r="D140" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F140" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C141">
         <v>4</v>
       </c>
       <c r="D141" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F141" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="142" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4673,234 +4667,234 @@
         <v>3</v>
       </c>
       <c r="D142" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E142" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F142" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C143">
         <v>4</v>
       </c>
       <c r="D143" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G143" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C144">
         <v>4</v>
       </c>
       <c r="D144" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F144" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C145">
         <v>4</v>
       </c>
       <c r="D145" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B146" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C146">
         <v>4</v>
       </c>
       <c r="D146" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C147">
         <v>5</v>
       </c>
       <c r="D147" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C148">
         <v>5</v>
       </c>
       <c r="D148" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C149">
         <v>5</v>
       </c>
       <c r="D149" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C150">
         <v>5</v>
       </c>
       <c r="D150" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F150" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C151">
         <v>5</v>
       </c>
       <c r="D151" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F151" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C152">
         <v>5</v>
       </c>
       <c r="D152" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F152" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C153">
         <v>5</v>
       </c>
       <c r="D153" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F153" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C154">
         <v>4</v>
       </c>
       <c r="F154" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G154" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C155">
         <v>4</v>
       </c>
       <c r="D155" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F155" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="156" spans="1:7" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4909,118 +4903,118 @@
         <v>3</v>
       </c>
       <c r="D156" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E156" s="21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F156" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C157">
         <v>4</v>
       </c>
       <c r="D157" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F157" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C158">
         <v>4</v>
       </c>
       <c r="D158" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F158" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C159">
         <v>4</v>
       </c>
       <c r="D159" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F159" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G159" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C160">
         <v>4</v>
       </c>
       <c r="D160" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F160" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C161">
         <v>4</v>
       </c>
       <c r="D161" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F161" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C162">
         <v>4</v>
       </c>
       <c r="D162" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F162" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="163" spans="1:6" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5032,10 +5026,10 @@
         <v>5</v>
       </c>
       <c r="E163" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F163" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="164" spans="1:6" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5044,149 +5038,149 @@
         <v>2</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E164" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F164" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C165">
         <v>3</v>
       </c>
       <c r="D165" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F165" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C166">
         <v>3</v>
       </c>
       <c r="D166" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F166" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C167">
         <v>3</v>
       </c>
       <c r="D167" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F167" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C168">
         <v>3</v>
       </c>
       <c r="D168" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F168" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C169">
         <v>3</v>
       </c>
       <c r="D169" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F169" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C170">
         <v>3</v>
       </c>
       <c r="D170" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F170" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C171">
         <v>3</v>
       </c>
       <c r="D171" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F171" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C172">
         <v>3</v>
       </c>
       <c r="D172" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F172" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="173" spans="1:6" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5195,64 +5189,64 @@
         <v>2</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E173" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F173" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C174">
         <v>3</v>
       </c>
       <c r="D174" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F174" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C175">
         <v>3</v>
       </c>
       <c r="D175" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F175" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C176">
         <v>3</v>
       </c>
       <c r="D176" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F176" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="177" spans="1:6" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5261,200 +5255,200 @@
         <v>2</v>
       </c>
       <c r="D177" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E177" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F177" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C178">
         <v>3</v>
       </c>
       <c r="D178" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F178" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C179">
         <v>3</v>
       </c>
       <c r="D179" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F179" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C180">
         <v>3</v>
       </c>
       <c r="D180" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F180" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="181" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C181">
         <v>3</v>
       </c>
       <c r="D181" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F181" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C182">
         <v>4</v>
       </c>
       <c r="D182" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F182" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C183">
         <v>4</v>
       </c>
       <c r="D183" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F183" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C184">
         <v>4</v>
       </c>
       <c r="D184" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F184" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C185">
         <v>4</v>
       </c>
       <c r="D185" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F185" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C186">
         <v>4</v>
       </c>
       <c r="D186" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F186" s="6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C187">
         <v>4</v>
       </c>
       <c r="D187" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F187" s="6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C188">
         <v>3</v>
       </c>
       <c r="D188" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F188" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="189" spans="1:6" s="14" customFormat="1" ht="68" x14ac:dyDescent="0.2">
@@ -5463,81 +5457,81 @@
         <v>2</v>
       </c>
       <c r="D189" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E189" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F189" s="20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C190">
         <v>3</v>
       </c>
       <c r="D190" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F190" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C191">
         <v>3</v>
       </c>
       <c r="D191" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F191" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C192">
         <v>3</v>
       </c>
       <c r="D192" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F192" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C193">
         <v>3</v>
       </c>
       <c r="D193" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F193" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="194" spans="1:6" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5546,115 +5540,115 @@
         <v>2</v>
       </c>
       <c r="D194" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E194" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F194" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C195">
         <v>3</v>
       </c>
       <c r="D195" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F195" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C196">
         <v>3</v>
       </c>
       <c r="D196" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F196" s="6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C197">
         <v>3</v>
       </c>
       <c r="D197" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F197" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C198">
         <v>3</v>
       </c>
       <c r="D198" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F198" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C199">
         <v>3</v>
       </c>
       <c r="D199" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F199" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C200">
         <v>3</v>
       </c>
       <c r="D200" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F200" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="201" spans="1:6" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5663,115 +5657,115 @@
         <v>2</v>
       </c>
       <c r="D201" s="15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E201" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F201" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C202">
         <v>3</v>
       </c>
       <c r="D202" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F202" s="6" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="203" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C203">
         <v>3</v>
       </c>
       <c r="D203" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F203" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C204">
         <v>3</v>
       </c>
       <c r="D204" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F204" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C205">
         <v>3</v>
       </c>
       <c r="D205" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F205" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C206">
         <v>3</v>
       </c>
       <c r="D206" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F206" s="6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C207">
         <v>3</v>
       </c>
       <c r="D207" s="11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F207" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="208" spans="1:6" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5783,10 +5777,10 @@
         <v>6</v>
       </c>
       <c r="E208" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F208" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="209" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5795,50 +5789,50 @@
         <v>2</v>
       </c>
       <c r="D209" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E209" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F209" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C210">
         <v>3</v>
       </c>
       <c r="D210" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F210" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C211">
         <v>3</v>
       </c>
       <c r="D211" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F211" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G211" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="212" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5847,33 +5841,33 @@
         <v>2</v>
       </c>
       <c r="D212" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E212" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F212" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C213">
         <v>3</v>
       </c>
       <c r="D213" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F213" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G213" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="214" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5882,30 +5876,30 @@
         <v>2</v>
       </c>
       <c r="D214" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E214" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F214" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="215" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C215">
         <v>3</v>
       </c>
       <c r="D215" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F215" s="6" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="216" spans="1:7" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5914,30 +5908,30 @@
         <v>2</v>
       </c>
       <c r="D216" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E216" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F216" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C217">
         <v>3</v>
       </c>
       <c r="D217" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F217" s="6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="218" spans="1:7" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5946,248 +5940,248 @@
         <v>1</v>
       </c>
       <c r="D218" s="13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E218" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F218" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C219">
         <v>2</v>
       </c>
       <c r="F219" s="6" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C220">
         <v>3</v>
       </c>
       <c r="D220" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F220" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="221" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C221">
         <v>3</v>
       </c>
       <c r="D221" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F221" s="6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="222" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B222" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C222">
         <v>3</v>
       </c>
       <c r="D222" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F222" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="223" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C223">
         <v>3</v>
       </c>
       <c r="D223" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F223" s="6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="224" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C224">
         <v>3</v>
       </c>
       <c r="D224" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F224" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C225">
         <v>3</v>
       </c>
       <c r="D225" s="13" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F225" s="6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C226">
         <v>3</v>
       </c>
       <c r="D226" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C227">
         <v>3</v>
       </c>
       <c r="D227" s="13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F227" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C228">
         <v>3</v>
       </c>
       <c r="D228" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F228" s="6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C229">
         <v>3</v>
       </c>
       <c r="D229" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F229" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="230" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C230">
         <v>3</v>
       </c>
       <c r="D230" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F230" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C231">
         <v>3</v>
       </c>
       <c r="D231" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F231" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C232">
         <v>3</v>
       </c>
       <c r="D232" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F232" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -6201,8 +6195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6001E7-1139-9540-9B4D-223FB26BDC60}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A7:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6224,35 +6218,35 @@
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>